<commit_message>
added for new scan
</commit_message>
<xml_diff>
--- a/digiverifier_backened/src/main/resources/BulkUanSearch.xlsx
+++ b/digiverifier_backened/src/main/resources/BulkUanSearch.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Applicant ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Talent Candidate ID</t>
   </si>
   <si>
     <t xml:space="preserve">UAN Number</t>
@@ -36,7 +39,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -59,16 +62,28 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -76,6 +91,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -102,7 +124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -113,6 +135,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -127,34 +153,144 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="15.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>